<commit_message>
add obq44 test and some changes on all files
</commit_message>
<xml_diff>
--- a/scoring/tests/WAQ/WAQ_test_1.xlsx
+++ b/scoring/tests/WAQ/WAQ_test_1.xlsx
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5">

</xml_diff>